<commit_message>
Fixed uncertainty for areal denisty and added uncertainty prop. for decay constant in calculations of bc and xs
</commit_message>
<xml_diff>
--- a/30MeV_Ti_Ni_Zr_Foils.xlsx
+++ b/30MeV_Ti_Ni_Zr_Foils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CD2EF24-C881-3944-90E4-8192613EDC09}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB50D176-0B8D-C04C-979D-536F412986DF}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +214,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -359,6 +365,9 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,6 +383,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,7 +691,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="89" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -14791,8 +14804,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14919,7 +14932,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>7.0251334506897453E-2</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="46">
         <f>M2/(G2*I2)*1000*100</f>
         <v>11.534860216590406</v>
       </c>
@@ -15149,7 +15162,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>7.0251334506897453E-2</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="46">
         <f>M8/(G8*I8)*1000*100</f>
         <v>11.739610776049215</v>
       </c>
@@ -15359,7 +15372,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>6.9751344073071458E-2</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="46">
         <f>M14/(G14*I14)*1000*100</f>
         <v>11.273409008046965</v>
       </c>
@@ -15569,7 +15582,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>7.0501773027350167E-2</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="46">
         <f>M20/(G20*I20)*1000*100</f>
         <v>11.098635270536583</v>
       </c>
@@ -15779,7 +15792,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="46">
         <f>M26/(G26*I26)*1000*100</f>
         <v>11.317352224957295</v>
       </c>
@@ -28904,8 +28917,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29032,7 +29045,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>0.14699999999999999</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="46">
         <f>M2/(G2*I2)*1000*100</f>
         <v>23.252539668225811</v>
       </c>
@@ -29264,7 +29277,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>0.14599999999999999</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="46">
         <f>M8/(G8*I8)*1000*100</f>
         <v>23.103254061280758</v>
       </c>
@@ -29480,7 +29493,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>0.14499999999999999</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="46">
         <f>M14/(G14*I14)*1000*100</f>
         <v>23.063708646265905</v>
       </c>
@@ -29690,7 +29703,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>0.14699999999999999</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="46">
         <f>M20/(G20*I20)*1000*100</f>
         <v>23.200992607259803</v>
       </c>
@@ -29900,7 +29913,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>0.14299999999999999</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="46">
         <f>M26/(G26*I26)*1000*100</f>
         <v>22.745674627801741</v>
       </c>
@@ -43025,7 +43038,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I have made a file to plot the xs in the zr foils together with talys calculations
</commit_message>
<xml_diff>
--- a/30MeV_Ti_Ni_Zr_Foils.xlsx
+++ b/30MeV_Ti_Ni_Zr_Foils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB50D176-0B8D-C04C-979D-536F412986DF}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405F761D-48EA-004E-B504-DD4D24683D96}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -691,8 +691,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -819,7 +819,7 @@
         <f t="array" ref="M2">SQRT(AVERAGE(L2:L5^2))</f>
         <v>9.9750939845196451E-2</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="46">
         <f>M2/(G2*I2)*1000*100</f>
         <v>16.142414012011891</v>
       </c>
@@ -1049,7 +1049,7 @@
         <f t="array" ref="M8">SQRT(AVERAGE(L8:L11^2))</f>
         <v>0.104</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="46">
         <f>M8/(G8*I8)*1000*100</f>
         <v>16.37837716634834</v>
       </c>
@@ -1259,7 +1259,7 @@
         <f t="array" ref="M14">SQRT(AVERAGE(L14:L17^2))</f>
         <v>0.1</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="46">
         <f>M14/(G14*I14)*1000*100</f>
         <v>16.140475826907704</v>
       </c>
@@ -1469,7 +1469,7 @@
         <f t="array" ref="M20">SQRT(AVERAGE(L20:L23^2))</f>
         <v>0.10225091686630491</v>
       </c>
-      <c r="N20" s="19">
+      <c r="N20" s="46">
         <f>M20/(G20*I20)*1000*100</f>
         <v>16.19482979975502</v>
       </c>
@@ -1679,7 +1679,7 @@
         <f t="array" ref="M26">SQRT(AVERAGE(L26:L29^2))</f>
         <v>0.10199999999999999</v>
       </c>
-      <c r="N26" s="19">
+      <c r="N26" s="46">
         <f>M26/(G26*I26)*1000*100</f>
         <v>16.400139754752058</v>
       </c>
@@ -14804,7 +14804,7 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
including files to read empire
</commit_message>
<xml_diff>
--- a/30MeV_Ti_Ni_Zr_Foils.xlsx
+++ b/30MeV_Ti_Ni_Zr_Foils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405F761D-48EA-004E-B504-DD4D24683D96}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="14_{7FE2433E-3551-A74B-8720-1D259C5F8435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{383C8731-3233-2744-9F7E-0B7F99D14D46}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36760" yWindow="5320" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zr" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="31">
   <si>
     <t>Shot</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>E3</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -264,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,6 +374,9 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,9 +399,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +439,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -536,7 +545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -678,7 +687,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -705,6 +714,7 @@
     <col min="8" max="8" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
     <col min="14" max="14" width="16.6640625" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" customWidth="1"/>
     <col min="16" max="16" width="8.83203125" customWidth="1"/>
@@ -794,7 +804,7 @@
       <c r="F2" s="15">
         <v>24.67</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="16" cm="1">
         <f t="array" ref="G2">SQRT(AVERAGE(F2:F5^2))</f>
         <v>24.725126895528767</v>
       </c>
@@ -854,19 +864,27 @@
       <c r="F3" s="15">
         <v>24.77</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="H3" s="16">
         <v>25.04</v>
       </c>
-      <c r="I3" s="16"/>
+      <c r="I3" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="J3" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="43" t="s">
+        <v>29</v>
+      </c>
       <c r="L3" s="18">
         <v>0.1</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="24" t="s">
+        <v>29</v>
+      </c>
       <c r="N3" s="19" t="s">
         <v>17</v>
       </c>
@@ -898,19 +916,31 @@
       <c r="F4" s="15">
         <v>24.83</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>9.1469484893414235E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>24.97</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>3.3040379335998495E-2</v>
+      </c>
       <c r="J4" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="18">
+        <f xml:space="preserve"> STDEV(J2:J5)</f>
+        <v>0</v>
+      </c>
       <c r="L4" s="18">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <f xml:space="preserve"> STDEV(L2:L5)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -931,7 +961,9 @@
       <c r="H5" s="16">
         <v>24.97</v>
       </c>
-      <c r="I5" s="16"/>
+      <c r="I5" s="47" t="s">
+        <v>30</v>
+      </c>
       <c r="J5" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1117,19 +1149,31 @@
       <c r="F10" s="15">
         <v>24.83</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>3.201562118716398E-2</v>
+      </c>
       <c r="H10" s="16">
         <v>25.58</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>6.9761498454854368E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="18">
+        <f>STDEV(J8:J11)</f>
+        <v>0</v>
+      </c>
       <c r="L10" s="18">
         <v>0.104</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <f>STDEV(L8:L11)</f>
+        <v>0</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -1234,7 +1278,7 @@
       <c r="F14" s="15">
         <v>25.01</v>
       </c>
-      <c r="G14" s="16">
+      <c r="G14" s="16" cm="1">
         <f t="array" ref="G14">SQRT(AVERAGE(F14:F17^2))</f>
         <v>25.015004497301216</v>
       </c>
@@ -1327,19 +1371,31 @@
       <c r="F16" s="15">
         <v>25</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>1.7320508075688062E-2</v>
+      </c>
       <c r="H16" s="16">
         <v>24.84</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>5.8523499553598569E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <f>STDEV(J14:J17)</f>
+        <v>0</v>
+      </c>
       <c r="L16" s="18">
         <v>0.1</v>
       </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="24">
+        <f>STDEV(L14:L17)</f>
+        <v>0</v>
+      </c>
       <c r="N16" s="19"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -1537,19 +1593,31 @@
       <c r="F22" s="15">
         <v>25.43</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>5.4390562906935364E-2</v>
+      </c>
       <c r="H22" s="16">
         <v>24.76</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>4.5000000000000387E-2</v>
+      </c>
       <c r="J22" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <f>STDEV(J20:J23)</f>
+        <v>0</v>
+      </c>
       <c r="L22" s="18">
         <v>0.10199999999999999</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="24">
+        <f>STDEV(L20:L23)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="N22" s="19"/>
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
@@ -1747,19 +1815,31 @@
       <c r="F28" s="15">
         <v>25.16</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>3.2015621187163973E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>24.65</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>4.425306015783894E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <f>STDEV(J26:J29)</f>
+        <v>0</v>
+      </c>
       <c r="L28" s="18">
         <v>0.10199999999999999</v>
       </c>
-      <c r="M28" s="24"/>
+      <c r="M28" s="24">
+        <f>STDEV(L26:L29)</f>
+        <v>0</v>
+      </c>
       <c r="N28" s="19"/>
       <c r="O28" s="25"/>
       <c r="P28" s="25"/>
@@ -14804,8 +14884,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15011,11 +15091,17 @@
       <c r="F4" s="15">
         <v>24.3</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>8.5780728216385188E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>25.13</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>4.9665548085838167E-2</v>
+      </c>
       <c r="J4" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
@@ -15023,7 +15109,10 @@
       <c r="L4" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <f>STDEV(L2:L5)</f>
+        <v>4.9999999999999351E-4</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -15230,11 +15319,17 @@
       <c r="F10" s="15">
         <v>24.36</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>4.1231056256177734E-2</v>
+      </c>
       <c r="H10" s="16">
         <v>24.5</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>6.4807406984078136E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
@@ -15242,7 +15337,10 @@
       <c r="L10" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <f>STDEV(L8:L11)</f>
+        <v>4.9999999999999351E-4</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -15440,19 +15538,31 @@
       <c r="F16" s="15">
         <v>24.57</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>4.19324854180309E-2</v>
+      </c>
       <c r="H16" s="16">
         <v>25.23</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>4.7609522856953058E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <f>STDEV(J14:J17)</f>
+        <v>4.9999999999999871E-4</v>
+      </c>
       <c r="L16" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M16" s="24"/>
+      <c r="M16" s="24">
+        <f>STDEV(L14:L17)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="N16" s="19"/>
       <c r="O16" s="25"/>
       <c r="P16" s="25"/>
@@ -15650,19 +15760,31 @@
       <c r="F22" s="15">
         <v>25.17</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>1.7320508075688745E-2</v>
+      </c>
       <c r="H22" s="16">
         <v>25.21</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>3.4034296427770241E-2</v>
+      </c>
       <c r="J22" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <f>STDEV(J20:J23)</f>
+        <v>4.9999999999999871E-4</v>
+      </c>
       <c r="L22" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="M22" s="24"/>
+      <c r="M22" s="24">
+        <f>STDEV(L20:L23)</f>
+        <v>5.7735026918961832E-4</v>
+      </c>
       <c r="N22" s="19"/>
       <c r="O22" s="25"/>
       <c r="P22" s="25"/>
@@ -15860,15 +15982,24 @@
       <c r="F28" s="15">
         <v>25.31</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>3.9475730941090879E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>24.75</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>5.259911279353055E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <f>STDEV(J26:J29)</f>
+        <v>4.9999999999999871E-4</v>
+      </c>
       <c r="L28" s="18">
         <v>7.0999999999999994E-2</v>
       </c>
@@ -28917,8 +29048,8 @@
   </sheetPr>
   <dimension ref="A1:AE1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29020,7 +29151,7 @@
       <c r="F2" s="15">
         <v>25.29</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="16" cm="1">
         <f t="array" ref="G2">SQRT(AVERAGE(F2:F5^2))</f>
         <v>25.282503337288418</v>
       </c>
@@ -29124,19 +29255,31 @@
       <c r="F4" s="15">
         <v>25.29</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="16">
+        <f>STDEV(F2:F5)</f>
+        <v>1.499999999999879E-2</v>
+      </c>
       <c r="H4" s="16">
         <v>25.01</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="16">
+        <f>STDEV(H2:H5)</f>
+        <v>5.77350269189716E-3</v>
+      </c>
       <c r="J4" s="17">
         <v>0.03</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="18">
+        <f>STDEV(J2:J5)</f>
+        <v>5.7735026918962428E-4</v>
+      </c>
       <c r="L4" s="18">
         <v>0.14699999999999999</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="24">
+        <f>STDEV(L2:L5)</f>
+        <v>0</v>
+      </c>
       <c r="N4" s="19"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
@@ -29351,19 +29494,31 @@
       <c r="F10" s="15">
         <v>25.01</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16">
+        <f>STDEV(F8:F11)</f>
+        <v>3.366501646120551E-2</v>
+      </c>
       <c r="H10" s="16">
         <v>25.22</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="16">
+        <f>STDEV(H8:H11)</f>
+        <v>2.6299556396765893E-2</v>
+      </c>
       <c r="J10" s="17">
         <v>0.03</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="18">
+        <f>STDEV(J8:J11)</f>
+        <v>5.7735026918962428E-4</v>
+      </c>
       <c r="L10" s="18">
         <v>0.14599999999999999</v>
       </c>
-      <c r="M10" s="24"/>
+      <c r="M10" s="24">
+        <f>STDEV(L8:L11)</f>
+        <v>0</v>
+      </c>
       <c r="N10" s="19"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
@@ -29561,15 +29716,24 @@
       <c r="F16" s="15">
         <v>25.07</v>
       </c>
-      <c r="G16" s="16"/>
+      <c r="G16" s="16">
+        <f>STDEV(F14:F17)</f>
+        <v>6.8495741960115139E-2</v>
+      </c>
       <c r="H16" s="16">
         <v>25.1</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="16">
+        <f>STDEV(H14:H17)</f>
+        <v>2.9999999999999357E-2</v>
+      </c>
       <c r="J16" s="17">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="K16" s="18"/>
+      <c r="K16" s="18">
+        <f>STDEV(J14:J17)</f>
+        <v>9.5742710775633744E-4</v>
+      </c>
       <c r="L16" s="43">
         <v>0.14499999999999999</v>
       </c>
@@ -29771,15 +29935,24 @@
       <c r="F22" s="15">
         <v>25.16</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="16">
+        <f>STDEV(F20:F23)</f>
+        <v>1.5000000000000567E-2</v>
+      </c>
       <c r="H22" s="16">
         <v>25.2</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="16">
+        <f>STDEV(H20:H23)</f>
+        <v>7.3484692283495065E-2</v>
+      </c>
       <c r="J22" s="17">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="K22" s="18"/>
+      <c r="K22" s="18">
+        <f>STDEV(J20:J23)</f>
+        <v>4.9999999999999871E-4</v>
+      </c>
       <c r="L22" s="18">
         <v>0.14699999999999999</v>
       </c>
@@ -29981,15 +30154,24 @@
       <c r="F28" s="15">
         <v>25.03</v>
       </c>
-      <c r="G28" s="16"/>
+      <c r="G28" s="16">
+        <f>STDEV(F26:F29)</f>
+        <v>1.2583057392117059E-2</v>
+      </c>
       <c r="H28" s="16">
         <v>25.1</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="16">
+        <f>STDEV(H26:H29)</f>
+        <v>1.6329931618554172E-2</v>
+      </c>
       <c r="J28" s="17">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="K28" s="18"/>
+      <c r="K28" s="18">
+        <f>STDEV(J26:J29)</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
       <c r="L28" s="18">
         <v>0.14299999999999999</v>
       </c>

</xml_diff>